<commit_message>
processing Batch 1 done
</commit_message>
<xml_diff>
--- a/pH_optode/Aug_20_Wadden_sea_B1.xlsx
+++ b/pH_optode/Aug_20_Wadden_sea_B1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_LAB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_LAB/Aug_20_Wadden_sea_B1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{91065B91-C42E-43FE-A7A7-3A2A7AA24902}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5C7E0EE3-0487-4BCF-80CB-71E2A913E9A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
+    <workbookView xWindow="28740" yWindow="780" windowWidth="21600" windowHeight="11265" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>CRM</t>
   </si>
   <si>
-    <t>2020-08-20_130648_20082020_CRM1</t>
-  </si>
-  <si>
     <t>28-07-2020</t>
   </si>
   <si>
@@ -116,52 +113,55 @@
     <t>buffer_2</t>
   </si>
   <si>
-    <t>2020-08-20_135157_20082020_B1S1</t>
-  </si>
-  <si>
-    <t>2020-08-20_142849_20082020_B1S2</t>
-  </si>
-  <si>
-    <t>2020-08-20_144520_20082020_B1S3</t>
-  </si>
-  <si>
-    <t>2020-08-20_150143_20082020_B1S4</t>
-  </si>
-  <si>
-    <t>2020-08-20_151832_20082020_B1S5</t>
-  </si>
-  <si>
-    <t>2020-08-20_153344_20082020_B1S6</t>
-  </si>
-  <si>
-    <t>2020-08-20_154832_20082020_B1S7</t>
-  </si>
-  <si>
-    <t>2020-08-20_160442_20082020_B1S8</t>
-  </si>
-  <si>
-    <t>2020-08-20_161906_20082020_B1S9</t>
-  </si>
-  <si>
-    <t>2020-08-20_163638_20082020_B1S10</t>
-  </si>
-  <si>
-    <t>2020-08-20_165122_20082020_B1S11</t>
-  </si>
-  <si>
-    <t>2020-08-20_170635_20082020_B1S12</t>
-  </si>
-  <si>
-    <t>2020-08-20_172206_20082020_B1S13</t>
-  </si>
-  <si>
-    <t>2020-08-20_173806_20082020_B1S14</t>
-  </si>
-  <si>
-    <t>2020-08-20_175237_20082020_B1S15</t>
-  </si>
-  <si>
-    <t>2020-08-20_182643_20082020_CRM2</t>
+    <t>20082020_CRM1</t>
+  </si>
+  <si>
+    <t>_20082020_B1S1</t>
+  </si>
+  <si>
+    <t>20082020_B1S2</t>
+  </si>
+  <si>
+    <t>20082020_B1S3</t>
+  </si>
+  <si>
+    <t>20082020_B1S4</t>
+  </si>
+  <si>
+    <t>20082020_B1S5</t>
+  </si>
+  <si>
+    <t>20082020_B1S6</t>
+  </si>
+  <si>
+    <t>20082020_B1S7</t>
+  </si>
+  <si>
+    <t>20082020_B1S8</t>
+  </si>
+  <si>
+    <t>20082020_B1S9</t>
+  </si>
+  <si>
+    <t>20082020_B1S10</t>
+  </si>
+  <si>
+    <t>20082020_B1S11</t>
+  </si>
+  <si>
+    <t>20082020_B1S12</t>
+  </si>
+  <si>
+    <t>20082020_B1S13</t>
+  </si>
+  <si>
+    <t>20082020_B1S14</t>
+  </si>
+  <si>
+    <t>20082020_B1S15</t>
+  </si>
+  <si>
+    <t>20082020_CRM2</t>
   </si>
 </sst>
 </file>
@@ -170,7 +170,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -672,16 +672,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1057,26 +1057,26 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" style="4" customWidth="1"/>
-    <col min="3" max="5" width="10.7265625" style="2"/>
-    <col min="6" max="6" width="10.7265625" style="5"/>
-    <col min="7" max="8" width="10.7265625" style="6"/>
-    <col min="9" max="9" width="10.7265625" style="5"/>
-    <col min="10" max="10" width="10.7265625" style="14"/>
-    <col min="11" max="13" width="10.7265625" style="2"/>
-    <col min="14" max="14" width="19.36328125" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="10.7265625" style="2"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="4" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="2"/>
+    <col min="6" max="6" width="10.7109375" style="5"/>
+    <col min="7" max="8" width="10.7109375" style="6"/>
+    <col min="9" max="9" width="10.7109375" style="5"/>
+    <col min="10" max="10" width="10.7109375" style="14"/>
+    <col min="11" max="13" width="10.7109375" style="2"/>
+    <col min="14" max="14" width="19.42578125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>10</v>
@@ -1094,10 +1094,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>4</v>
@@ -1118,7 +1118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1138,13 +1138,13 @@
         <v>7</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>13</v>
@@ -1162,9 +1162,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4">
         <v>44063</v>
@@ -1191,12 +1191,12 @@
         <v>8.35</v>
       </c>
       <c r="J3" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>44063</v>
@@ -1226,9 +1226,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="13">
         <v>44063</v>
@@ -1258,9 +1258,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="13">
         <v>44063</v>
@@ -1290,9 +1290,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="13">
         <v>44063</v>
@@ -1322,9 +1322,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="13">
         <v>44063</v>
@@ -1354,9 +1354,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="13">
         <v>44063</v>
@@ -1387,9 +1387,9 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="13">
         <v>44063</v>
@@ -1420,9 +1420,9 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="13">
         <v>44063</v>
@@ -1453,9 +1453,9 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="13">
         <v>44063</v>
@@ -1486,9 +1486,9 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="13">
         <v>44063</v>
@@ -1518,9 +1518,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="13">
         <v>44063</v>
@@ -1550,9 +1550,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="13">
         <v>44063</v>
@@ -1582,9 +1582,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="13">
         <v>44063</v>
@@ -1614,9 +1614,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="13">
         <v>44063</v>
@@ -1646,9 +1646,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="13">
         <v>44063</v>
@@ -1678,9 +1678,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="13">
         <v>44063</v>
@@ -1717,21 +1717,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027E85BF46FFBA5448F68919BA489A1DA" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="45a9c6a0386fdd3966398fc659f672bc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211" xmlns:ns4="1e11a0bb-5c52-4e83-8dd3-aa81c1705742" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5fd16eb0bef241ffc3cb418196d56410" ns3:_="" ns4:_="">
     <xsd:import namespace="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211"/>
@@ -1954,24 +1939,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E16F44-C68D-4E79-A4BA-87CF7924D4A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77FFA200-F0B2-4031-AD08-862C0DB7F006}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46B2F9E1-9454-4E0C-80CD-4240C2750498}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1988,4 +1971,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77FFA200-F0B2-4031-AD08-862C0DB7F006}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E16F44-C68D-4E79-A4BA-87CF7924D4A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>